<commit_message>
TS measurements for rf-dfs board
</commit_message>
<xml_diff>
--- a/Tangential Sensitivity Report/Figures/Data/TanSensADL5902.xlsx
+++ b/Tangential Sensitivity Report/Figures/Data/TanSensADL5902.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remyv\Documents\NRAO\Solar Telescope Redesign\Tangential Sensitivity Report\Figures\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D380B86-7C26-48A0-85DA-100DF07A2C52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4028A1-3987-4B6F-AD7E-833DF593DE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{D7E56B31-A8C5-4C1C-8899-29094027D379}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D7E56B31-A8C5-4C1C-8899-29094027D379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Freq (GHz)</t>
   </si>
@@ -34,6 +45,9 @@
   </si>
   <si>
     <t>ZX60-83LN-S+</t>
+  </si>
+  <si>
+    <t>RF-DFS-6G</t>
   </si>
 </sst>
 </file>
@@ -69,9 +83,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,18 +402,18 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C24"/>
+      <selection activeCell="D1" sqref="D1:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,9 +423,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -422,8 +437,11 @@
       <c r="C2">
         <v>-59</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+0.5</f>
         <v>2.5</v>
@@ -434,8 +452,11 @@
       <c r="C3">
         <v>-59</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>-59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+0.5</f>
         <v>3</v>
@@ -446,8 +467,11 @@
       <c r="C4">
         <v>-59</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>-57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3.5</v>
@@ -458,8 +482,11 @@
       <c r="C5">
         <v>-56</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>-49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -470,8 +497,11 @@
       <c r="C6">
         <v>-55</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>-47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>4.5</v>
@@ -482,8 +512,11 @@
       <c r="C7">
         <v>-53</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -494,8 +527,11 @@
       <c r="C8">
         <v>-51</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>5.5</v>
@@ -506,8 +542,11 @@
       <c r="C9">
         <v>-49</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -518,8 +557,11 @@
       <c r="C10">
         <v>-45</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6.5</v>
@@ -530,8 +572,11 @@
       <c r="C11">
         <v>-40</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>-22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -542,8 +587,11 @@
       <c r="C12">
         <v>-36</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>A12+0.25</f>
         <v>7.25</v>
@@ -554,8 +602,11 @@
       <c r="C13">
         <v>-34</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" ref="A14:A24" si="1">A13+0.25</f>
         <v>7.5</v>
@@ -566,8 +617,11 @@
       <c r="C14">
         <v>-32</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>7.75</v>
@@ -578,8 +632,11 @@
       <c r="C15">
         <v>-30</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -590,8 +647,11 @@
       <c r="C16">
         <v>-28</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>8.25</v>
@@ -602,8 +662,11 @@
       <c r="C17">
         <v>-26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>8.5</v>
@@ -614,8 +677,11 @@
       <c r="C18">
         <v>-24</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>8.75</v>
@@ -626,8 +692,11 @@
       <c r="C19">
         <v>-22</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -638,8 +707,11 @@
       <c r="C20">
         <v>-20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>9.25</v>
@@ -650,8 +722,11 @@
       <c r="C21">
         <v>-18</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>9.5</v>
@@ -662,8 +737,11 @@
       <c r="C22">
         <v>-16</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>9.75</v>
@@ -674,8 +752,11 @@
       <c r="C23">
         <v>-15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -685,6 +766,9 @@
       </c>
       <c r="C24">
         <v>-14</v>
+      </c>
+      <c r="D24">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>